<commit_message>
finished edit article, added test for tags & wrote testng.xml to run all tests together
</commit_message>
<xml_diff>
--- a/src/test/java/dataProvider/article/EditArticle.xlsx
+++ b/src/test/java/dataProvider/article/EditArticle.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="editNewArticleTest" sheetId="1" r:id="rId1"/>
@@ -415,8 +415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,7 +511,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="A1:G2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,6 +592,7 @@
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>